<commit_message>
Appeneded 4 rows to the RTM report
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$N$40</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirement_Traceability_Matrix!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -536,6 +536,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with the current status of the functional requirement.</t>
     </r>
@@ -548,6 +549,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>:  This column should be populated with a description of the technical assumption or customer need linked to the functional requirement.</t>
     </r>
@@ -560,6 +562,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with a description of the functional requirement.</t>
     </r>
@@ -572,6 +575,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>:  This column should be populated with a description of the architectural/design document linked to the functional requirement.</t>
     </r>
@@ -584,6 +588,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with a description of the technical specification linked to the functional requirement.</t>
     </r>
@@ -609,6 +614,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with a description of the software module(s) linked to the functional requirement.</t>
     </r>
@@ -621,6 +627,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with the test case number linked to the functional requirement.</t>
     </r>
@@ -633,6 +640,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with the module that the functional requirement has been tested in.</t>
     </r>
@@ -645,6 +653,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with the module that the functional requirement has been implemented in.</t>
     </r>
@@ -657,6 +666,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with a description of the verification document linked to the functional requirement.</t>
     </r>
@@ -669,6 +679,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should be populated with any additional comments</t>
     </r>
@@ -687,6 +698,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: This column should contain the ID of any associated utilities used for requirements tracking such as a repository, pipeline document, etc.</t>
     </r>
@@ -699,12 +711,25 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: A unique ID number used to identify the traceability item in the requirements traceability matrix.</t>
     </r>
   </si>
   <si>
     <t>National Center:</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
   </si>
 </sst>
 </file>
@@ -712,9 +737,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -793,13 +818,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1272,7 +1290,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1281,7 +1299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,7 +1342,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1369,7 +1387,7 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1390,13 +1408,13 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1417,7 +1435,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1957,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2766,6 +2784,31 @@
       <c r="L40" s="40"/>
       <c r="M40" s="40"/>
       <c r="N40" s="49"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="18" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>